<commit_message>
atur format tanggal pendataan
</commit_message>
<xml_diff>
--- a/public/Nominatif Pendaftaran PTSL Desa Sidomekar.xlsx
+++ b/public/Nominatif Pendaftaran PTSL Desa Sidomekar.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90">
   <si>
     <t>No Nominatif</t>
   </si>
@@ -228,6 +228,63 @@
   </si>
   <si>
     <t>Koordinator</t>
+  </si>
+  <si>
+    <t>12-02-2023</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>ISLAM</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>13-02-2023</t>
+  </si>
+  <si>
+    <t>BETENG</t>
+  </si>
+  <si>
+    <t>SIDOMEKAR</t>
+  </si>
+  <si>
+    <t>SEMBORO</t>
+  </si>
+  <si>
+    <t>YASAN</t>
+  </si>
+  <si>
+    <t>PEKARANGAN</t>
+  </si>
+  <si>
+    <t>EDI SANTOSO</t>
+  </si>
+  <si>
+    <t>SLAMET</t>
+  </si>
+  <si>
+    <t>3509070902670003</t>
+  </si>
+  <si>
+    <t>PERANGKAT DESA</t>
+  </si>
+  <si>
+    <t>DUSUN BETENG RT 004 RW 004 DESA SIDOMEKAR KECAMATAN SEMBORO</t>
+  </si>
+  <si>
+    <t>BUDIONO</t>
+  </si>
+  <si>
+    <t>3509071011790003</t>
+  </si>
+  <si>
+    <t>WIRASWASTA</t>
+  </si>
+  <si>
+    <t>DUSUN BETENG RT 002 RW 008 DESA SIDOMEKAR KECAMATAN SEMBORO</t>
   </si>
 </sst>
 </file>
@@ -563,7 +620,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:BS1"/>
+  <dimension ref="A1:BS2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -784,6 +841,137 @@
       </c>
       <c r="BS1" t="s">
         <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:71">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2" t="s">
+        <v>71</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2"/>
+      <c r="R2" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2"/>
+      <c r="T2" t="s">
+        <v>74</v>
+      </c>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2" t="s">
+        <v>75</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+      <c r="BE2"/>
+      <c r="BF2" t="s">
+        <v>81</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BJ2">
+        <v>55</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>73</v>
+      </c>
+      <c r="BP2">
+        <v>43</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>